<commit_message>
fix bug #105564, #105565
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.ctx/function/nts.uk.ctx.at.function.infra/src/main/resources/report/年間勤務表.xlsx
+++ b/nts.uk/uk.at/at.ctx/function/nts.uk.ctx.at.function.infra/src/main/resources/report/年間勤務表.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NITTSU\PJ\KWR008\nts.uk\uk.at\at.ctx\function\nts.uk.ctx.at.function.infra\src\main\resources\report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\01. UK\02.UkPersonInfo\SourceTreee\nts.uk\uk.at\at.ctx\function\nts.uk.ctx.at.function.infra\src\main\resources\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -35,6 +35,7 @@
     <definedName name="employeeRange">'★年間勤務表（1ヶ月）'!$A$5:$Z$14</definedName>
     <definedName name="employmentName">'★年間勤務表（1ヶ月）'!$A$6</definedName>
     <definedName name="empName">'★年間勤務表（1ヶ月）'!$A$5</definedName>
+    <definedName name="headerRange">'★年間勤務表（1ヶ月）'!$A$2:$Z$3</definedName>
     <definedName name="item">'★年間勤務表（1ヶ月）'!$C$5</definedName>
     <definedName name="jobTitle">'★年間勤務表（1ヶ月）'!$A$7</definedName>
     <definedName name="kkkk" localSheetId="0" hidden="1">#REF!</definedName>
@@ -83,6 +84,8 @@
     <definedName name="period5th">'★年間勤務表（1ヶ月）'!$X$5</definedName>
     <definedName name="period6th">'★年間勤務表（1ヶ月）'!$Y$5</definedName>
     <definedName name="period7th">'★年間勤務表（1ヶ月）'!$Z$5</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'★年間勤務表（1ヶ月）'!$A$1:$Z$14</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">'★年間勤務表（1ヶ月）'!$1:$3</definedName>
     <definedName name="sum">'★年間勤務表（1ヶ月）'!$Q$5</definedName>
     <definedName name="workplace">'★年間勤務表（1ヶ月）'!$A$4</definedName>
     <definedName name="workplaceRange">'★年間勤務表（1ヶ月）'!$A$4:$Z$14</definedName>
@@ -140,12 +143,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="6">
-    <numFmt numFmtId="176" formatCode="#,##0;\-#,##0;&quot;-&quot;"/>
-    <numFmt numFmtId="177" formatCode="_-&quot;｣&quot;* #,##0_-;\-&quot;｣&quot;* #,##0_-;_-&quot;｣&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_-&quot;｣&quot;* #,##0.00_-;\-&quot;｣&quot;* #,##0.00_-;_-&quot;｣&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="0.000%"/>
-    <numFmt numFmtId="180" formatCode="&quot;$&quot;#,\);\(&quot;$&quot;#,##0\)"/>
-    <numFmt numFmtId="181" formatCode="#,##0.00&quot; $&quot;;\-#,##0.00&quot; $&quot;"/>
+    <numFmt numFmtId="164" formatCode="#,##0;\-#,##0;&quot;-&quot;"/>
+    <numFmt numFmtId="165" formatCode="_-&quot;｣&quot;* #,##0_-;\-&quot;｣&quot;* #,##0_-;_-&quot;｣&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="_-&quot;｣&quot;* #,##0.00_-;\-&quot;｣&quot;* #,##0.00_-;_-&quot;｣&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="167" formatCode="0.000%"/>
+    <numFmt numFmtId="168" formatCode="&quot;$&quot;#,\);\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="169" formatCode="#,##0.00&quot; $&quot;;\-#,##0.00&quot; $&quot;"/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -295,7 +298,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -303,7 +306,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -628,9 +631,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
-    <xf numFmtId="179" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="180" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0">
       <alignment horizontal="left"/>
     </xf>
@@ -645,7 +648,7 @@
     <xf numFmtId="1" fontId="13" fillId="0" borderId="0" applyProtection="0">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="181" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="169" fontId="14" fillId="0" borderId="0"/>
     <xf numFmtId="10" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="4" fontId="10" fillId="0" borderId="0">
       <alignment horizontal="right"/>
@@ -660,8 +663,8 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="177" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="178" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -1280,7 +1283,7 @@
   <dimension ref="A1:AA25"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection sqref="A1:E1"/>
+      <selection activeCell="A2" sqref="A2:Z3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.140625" defaultRowHeight="15" customHeight="1"/>
@@ -1992,7 +1995,7 @@
   <phoneticPr fontId="3"/>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.39370078740157499" right="0.39370078740157499" top="0.98425196850393704" bottom="0.39370078740157499" header="0.39370078740157499" footer="0.31496062992126"/>
-  <pageSetup paperSize="9" scale="95" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="91" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;"MSゴシック,Regular"あいうえおあいうえおあいうえおあ株式会社
 &amp;C&amp;"MSゴシック,Regular"&amp;16★年間勤務表（1ヶ月）&amp;R&amp;"MSゴシック,Regular"&amp;D　&amp;T　

</xml_diff>

<commit_message>
KWR008: #129969: Exception khi số page trên sheet lớn hơn 1024
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.ctx/function/nts.uk.ctx.at.function.infra/src/main/resources/report/年間勤務表.xlsx
+++ b/nts.uk/uk.at/at.ctx/function/nts.uk.ctx.at.function.infra/src/main/resources/report/年間勤務表.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\01. UK\02.UkPersonInfo\SourceTreee\nts.uk\uk.at\at.ctx\function\nts.uk.ctx.at.function.infra\src\main\resources\report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NITTSU\PJ\Salary\nts.uk\uk.at\at.ctx\function\nts.uk.ctx.at.function.infra\src\main\resources\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -32,10 +32,10 @@
     <definedName name="def" localSheetId="0" hidden="1">{#N/A,#N/A,TRUE,"Sheet2";#N/A,#N/A,TRUE,"Sheet3";#N/A,#N/A,TRUE,"Sheet4";#N/A,#N/A,TRUE,"Sheet1"}</definedName>
     <definedName name="def" hidden="1">{#N/A,#N/A,TRUE,"Sheet2";#N/A,#N/A,TRUE,"Sheet3";#N/A,#N/A,TRUE,"Sheet4";#N/A,#N/A,TRUE,"Sheet1"}</definedName>
     <definedName name="empInfoLabel">'★年間勤務表（1ヶ月）'!$A$3</definedName>
-    <definedName name="employeeRange">'★年間勤務表（1ヶ月）'!$A$5:$Z$14</definedName>
+    <definedName name="employeeRange">'★年間勤務表（1ヶ月）'!$A$5:$Y$14</definedName>
     <definedName name="employmentName">'★年間勤務表（1ヶ月）'!$A$6</definedName>
     <definedName name="empName">'★年間勤務表（1ヶ月）'!$A$5</definedName>
-    <definedName name="headerRange">'★年間勤務表（1ヶ月）'!$A$2:$Z$3</definedName>
+    <definedName name="headerRange">'★年間勤務表（1ヶ月）'!$A$2:$Y$3</definedName>
     <definedName name="item">'★年間勤務表（1ヶ月）'!$C$5</definedName>
     <definedName name="jobTitle">'★年間勤務表（1ヶ月）'!$A$7</definedName>
     <definedName name="kkkk" localSheetId="0" hidden="1">#REF!</definedName>
@@ -71,7 +71,7 @@
     <definedName name="monthPeriodLabel4">'★年間勤務表（1ヶ月）'!$W$3</definedName>
     <definedName name="monthPeriodLabel5">'★年間勤務表（1ヶ月）'!$X$3</definedName>
     <definedName name="monthPeriodLabel6">'★年間勤務表（1ヶ月）'!$Y$3</definedName>
-    <definedName name="monthPeriodLabel7">'★年間勤務表（1ヶ月）'!$Z$3</definedName>
+    <definedName name="monthPeriodLabel7">'★年間勤務表（1ヶ月）'!#REF!</definedName>
     <definedName name="numExceedTime">'★年間勤務表（1ヶ月）'!$R$5</definedName>
     <definedName name="numExceedTime1">'★年間勤務表（1ヶ月）'!$R$5</definedName>
     <definedName name="numRemainingTime">'★年間勤務表（1ヶ月）'!$S$5</definedName>
@@ -83,12 +83,12 @@
     <definedName name="period4th">'★年間勤務表（1ヶ月）'!$W$5</definedName>
     <definedName name="period5th">'★年間勤務表（1ヶ月）'!$X$5</definedName>
     <definedName name="period6th">'★年間勤務表（1ヶ月）'!$Y$5</definedName>
-    <definedName name="period7th">'★年間勤務表（1ヶ月）'!$Z$5</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'★年間勤務表（1ヶ月）'!$A$1:$Z$14</definedName>
+    <definedName name="period7th">'★年間勤務表（1ヶ月）'!#REF!</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'★年間勤務表（1ヶ月）'!$A$1:$Y$14</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'★年間勤務表（1ヶ月）'!$1:$3</definedName>
     <definedName name="sum">'★年間勤務表（1ヶ月）'!$Q$5</definedName>
     <definedName name="workplace">'★年間勤務表（1ヶ月）'!$A$4</definedName>
-    <definedName name="workplaceRange">'★年間勤務表（1ヶ月）'!$A$4:$Z$14</definedName>
+    <definedName name="workplaceRange">'★年間勤務表（1ヶ月）'!$A$4:$Y$14</definedName>
     <definedName name="wrn.MIND." localSheetId="0" hidden="1">{#N/A,#N/A,TRUE,"Sheet2";#N/A,#N/A,TRUE,"Sheet3";#N/A,#N/A,TRUE,"Sheet4";#N/A,#N/A,TRUE,"Sheet1"}</definedName>
     <definedName name="wrn.MIND." hidden="1">{#N/A,#N/A,TRUE,"Sheet2";#N/A,#N/A,TRUE,"Sheet3";#N/A,#N/A,TRUE,"Sheet4";#N/A,#N/A,TRUE,"Sheet1"}</definedName>
     <definedName name="あああ" localSheetId="0" hidden="1">{#N/A,#N/A,TRUE,"Sheet2";#N/A,#N/A,TRUE,"Sheet3";#N/A,#N/A,TRUE,"Sheet4";#N/A,#N/A,TRUE,"Sheet1"}</definedName>
@@ -143,12 +143,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="6">
-    <numFmt numFmtId="164" formatCode="#,##0;\-#,##0;&quot;-&quot;"/>
-    <numFmt numFmtId="165" formatCode="_-&quot;｣&quot;* #,##0_-;\-&quot;｣&quot;* #,##0_-;_-&quot;｣&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="_-&quot;｣&quot;* #,##0.00_-;\-&quot;｣&quot;* #,##0.00_-;_-&quot;｣&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="167" formatCode="0.000%"/>
-    <numFmt numFmtId="168" formatCode="&quot;$&quot;#,\);\(&quot;$&quot;#,##0\)"/>
-    <numFmt numFmtId="169" formatCode="#,##0.00&quot; $&quot;;\-#,##0.00&quot; $&quot;"/>
+    <numFmt numFmtId="176" formatCode="#,##0;\-#,##0;&quot;-&quot;"/>
+    <numFmt numFmtId="177" formatCode="_-&quot;｣&quot;* #,##0_-;\-&quot;｣&quot;* #,##0_-;_-&quot;｣&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-&quot;｣&quot;* #,##0.00_-;\-&quot;｣&quot;* #,##0.00_-;_-&quot;｣&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="0.000%"/>
+    <numFmt numFmtId="180" formatCode="&quot;$&quot;#,\);\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="181" formatCode="#,##0.00&quot; $&quot;;\-#,##0.00&quot; $&quot;"/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -298,7 +298,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -306,7 +306,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -631,9 +631,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
+    <xf numFmtId="179" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="180" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0">
       <alignment horizontal="left"/>
     </xf>
@@ -648,7 +648,7 @@
     <xf numFmtId="1" fontId="13" fillId="0" borderId="0" applyProtection="0">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="169" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="181" fontId="14" fillId="0" borderId="0"/>
     <xf numFmtId="10" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="4" fontId="10" fillId="0" borderId="0">
       <alignment horizontal="right"/>
@@ -663,8 +663,8 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="177" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="178" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -1280,10 +1280,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA25"/>
+  <dimension ref="A1:Z25"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:Z3"/>
+      <selection activeCell="A2" sqref="A2:Y3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.140625" defaultRowHeight="15" customHeight="1"/>
@@ -1294,11 +1294,10 @@
     <col min="15" max="17" width="5.42578125" style="2" customWidth="1"/>
     <col min="18" max="19" width="3.7109375" style="2" customWidth="1"/>
     <col min="20" max="25" width="5.42578125" style="1" customWidth="1"/>
-    <col min="26" max="26" width="5.42578125" style="2" customWidth="1"/>
-    <col min="27" max="16384" width="3.140625" style="2"/>
+    <col min="26" max="16384" width="3.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="15" customHeight="1" thickBot="1">
+    <row r="1" spans="1:26" ht="15" customHeight="1" thickBot="1">
       <c r="A1" s="43"/>
       <c r="B1" s="44"/>
       <c r="C1" s="44"/>
@@ -1320,7 +1319,7 @@
       <c r="X1" s="4"/>
       <c r="Y1" s="4"/>
     </row>
-    <row r="2" spans="1:27" ht="15" customHeight="1">
+    <row r="2" spans="1:26" ht="15" customHeight="1">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="8"/>
@@ -1353,11 +1352,10 @@
       <c r="V2" s="14"/>
       <c r="W2" s="14"/>
       <c r="X2" s="14"/>
-      <c r="Y2" s="14"/>
-      <c r="Z2" s="15"/>
-      <c r="AA2" s="38"/>
-    </row>
-    <row r="3" spans="1:27" ht="15" customHeight="1" thickBot="1">
+      <c r="Y2" s="15"/>
+      <c r="Z2" s="38"/>
+    </row>
+    <row r="3" spans="1:26" ht="15" customHeight="1" thickBot="1">
       <c r="A3" s="51"/>
       <c r="B3" s="51"/>
       <c r="C3" s="37"/>
@@ -1388,11 +1386,10 @@
       <c r="V3" s="16"/>
       <c r="W3" s="16"/>
       <c r="X3" s="16"/>
-      <c r="Y3" s="16"/>
-      <c r="Z3" s="17"/>
-      <c r="AA3" s="38"/>
-    </row>
-    <row r="4" spans="1:27" ht="15" customHeight="1" thickBot="1">
+      <c r="Y3" s="17"/>
+      <c r="Z3" s="38"/>
+    </row>
+    <row r="4" spans="1:26" ht="15" customHeight="1" thickBot="1">
       <c r="A4" s="45"/>
       <c r="B4" s="46"/>
       <c r="C4" s="46"/>
@@ -1418,9 +1415,8 @@
       <c r="W4" s="20"/>
       <c r="X4" s="20"/>
       <c r="Y4" s="20"/>
-      <c r="Z4" s="18"/>
-    </row>
-    <row r="5" spans="1:27" ht="15" customHeight="1">
+    </row>
+    <row r="5" spans="1:26" ht="15" customHeight="1">
       <c r="A5" s="52"/>
       <c r="B5" s="53"/>
       <c r="C5" s="40"/>
@@ -1446,9 +1442,8 @@
       <c r="W5" s="41"/>
       <c r="X5" s="41"/>
       <c r="Y5" s="41"/>
-      <c r="Z5" s="41"/>
-    </row>
-    <row r="6" spans="1:27" ht="15" customHeight="1">
+    </row>
+    <row r="6" spans="1:26" ht="15" customHeight="1">
       <c r="A6" s="48"/>
       <c r="B6" s="49"/>
       <c r="C6" s="23"/>
@@ -1474,9 +1469,8 @@
       <c r="W6" s="6"/>
       <c r="X6" s="6"/>
       <c r="Y6" s="6"/>
-      <c r="Z6" s="6"/>
-    </row>
-    <row r="7" spans="1:27" ht="15" customHeight="1">
+    </row>
+    <row r="7" spans="1:26" ht="15" customHeight="1">
       <c r="A7" s="48"/>
       <c r="B7" s="50"/>
       <c r="C7" s="24"/>
@@ -1502,9 +1496,8 @@
       <c r="W7" s="3"/>
       <c r="X7" s="3"/>
       <c r="Y7" s="3"/>
-      <c r="Z7" s="3"/>
-    </row>
-    <row r="8" spans="1:27" ht="15" customHeight="1">
+    </row>
+    <row r="8" spans="1:26" ht="15" customHeight="1">
       <c r="A8" s="29"/>
       <c r="B8" s="30"/>
       <c r="C8" s="25"/>
@@ -1530,9 +1523,8 @@
       <c r="W8" s="6"/>
       <c r="X8" s="6"/>
       <c r="Y8" s="6"/>
-      <c r="Z8" s="6"/>
-    </row>
-    <row r="9" spans="1:27" ht="15" customHeight="1">
+    </row>
+    <row r="9" spans="1:26" ht="15" customHeight="1">
       <c r="A9" s="29"/>
       <c r="B9" s="30"/>
       <c r="C9" s="26"/>
@@ -1558,9 +1550,8 @@
       <c r="W9" s="3"/>
       <c r="X9" s="3"/>
       <c r="Y9" s="3"/>
-      <c r="Z9" s="3"/>
-    </row>
-    <row r="10" spans="1:27" ht="15" customHeight="1">
+    </row>
+    <row r="10" spans="1:26" ht="15" customHeight="1">
       <c r="A10" s="29"/>
       <c r="B10" s="30"/>
       <c r="C10" s="25"/>
@@ -1586,9 +1577,8 @@
       <c r="W10" s="6"/>
       <c r="X10" s="6"/>
       <c r="Y10" s="6"/>
-      <c r="Z10" s="6"/>
-    </row>
-    <row r="11" spans="1:27" ht="15" customHeight="1">
+    </row>
+    <row r="11" spans="1:26" ht="15" customHeight="1">
       <c r="A11" s="29"/>
       <c r="B11" s="30"/>
       <c r="C11" s="26"/>
@@ -1614,9 +1604,8 @@
       <c r="W11" s="3"/>
       <c r="X11" s="3"/>
       <c r="Y11" s="3"/>
-      <c r="Z11" s="3"/>
-    </row>
-    <row r="12" spans="1:27" ht="15" customHeight="1">
+    </row>
+    <row r="12" spans="1:26" ht="15" customHeight="1">
       <c r="A12" s="29"/>
       <c r="B12" s="30"/>
       <c r="C12" s="25"/>
@@ -1642,9 +1631,8 @@
       <c r="W12" s="6"/>
       <c r="X12" s="6"/>
       <c r="Y12" s="6"/>
-      <c r="Z12" s="6"/>
-    </row>
-    <row r="13" spans="1:27" ht="15" customHeight="1">
+    </row>
+    <row r="13" spans="1:26" ht="15" customHeight="1">
       <c r="A13" s="29"/>
       <c r="B13" s="30"/>
       <c r="C13" s="26"/>
@@ -1670,9 +1658,8 @@
       <c r="W13" s="3"/>
       <c r="X13" s="3"/>
       <c r="Y13" s="3"/>
-      <c r="Z13" s="3"/>
-    </row>
-    <row r="14" spans="1:27" ht="15" customHeight="1" thickBot="1">
+    </row>
+    <row r="14" spans="1:26" ht="15" customHeight="1" thickBot="1">
       <c r="A14" s="28"/>
       <c r="B14" s="31"/>
       <c r="C14" s="27"/>
@@ -1698,12 +1685,11 @@
       <c r="W14" s="7"/>
       <c r="X14" s="7"/>
       <c r="Y14" s="7"/>
-      <c r="Z14" s="7"/>
-    </row>
-    <row r="15" spans="1:27" ht="15" customHeight="1">
+    </row>
+    <row r="15" spans="1:26" ht="15" customHeight="1">
       <c r="E15" s="39"/>
     </row>
-    <row r="16" spans="1:27" ht="15" customHeight="1">
+    <row r="16" spans="1:26" ht="15" customHeight="1">
       <c r="A16" s="36"/>
       <c r="B16" s="36"/>
       <c r="C16" s="36"/>
@@ -1729,9 +1715,8 @@
       <c r="W16" s="36"/>
       <c r="X16" s="36"/>
       <c r="Y16" s="36"/>
-      <c r="Z16" s="36"/>
-    </row>
-    <row r="17" spans="1:26" ht="15" customHeight="1">
+    </row>
+    <row r="17" spans="1:25" ht="15" customHeight="1">
       <c r="A17" s="36"/>
       <c r="B17" s="36"/>
       <c r="C17" s="36"/>
@@ -1757,9 +1742,8 @@
       <c r="W17" s="36"/>
       <c r="X17" s="36"/>
       <c r="Y17" s="36"/>
-      <c r="Z17" s="36"/>
-    </row>
-    <row r="18" spans="1:26" ht="15" customHeight="1">
+    </row>
+    <row r="18" spans="1:25" ht="15" customHeight="1">
       <c r="A18" s="36"/>
       <c r="B18" s="36"/>
       <c r="C18" s="36"/>
@@ -1785,9 +1769,8 @@
       <c r="W18" s="36"/>
       <c r="X18" s="36"/>
       <c r="Y18" s="36"/>
-      <c r="Z18" s="36"/>
-    </row>
-    <row r="19" spans="1:26" ht="15" customHeight="1">
+    </row>
+    <row r="19" spans="1:25" ht="15" customHeight="1">
       <c r="A19" s="36"/>
       <c r="B19" s="36"/>
       <c r="C19" s="36"/>
@@ -1813,9 +1796,8 @@
       <c r="W19" s="36"/>
       <c r="X19" s="36"/>
       <c r="Y19" s="36"/>
-      <c r="Z19" s="36"/>
-    </row>
-    <row r="20" spans="1:26" ht="15" customHeight="1">
+    </row>
+    <row r="20" spans="1:25" ht="15" customHeight="1">
       <c r="A20" s="36"/>
       <c r="B20" s="36"/>
       <c r="C20" s="36"/>
@@ -1841,9 +1823,8 @@
       <c r="W20" s="36"/>
       <c r="X20" s="36"/>
       <c r="Y20" s="36"/>
-      <c r="Z20" s="36"/>
-    </row>
-    <row r="21" spans="1:26" ht="15" customHeight="1">
+    </row>
+    <row r="21" spans="1:25" ht="15" customHeight="1">
       <c r="A21" s="36"/>
       <c r="B21" s="36"/>
       <c r="C21" s="36"/>
@@ -1869,9 +1850,8 @@
       <c r="W21" s="36"/>
       <c r="X21" s="36"/>
       <c r="Y21" s="36"/>
-      <c r="Z21" s="36"/>
-    </row>
-    <row r="22" spans="1:26" ht="15" customHeight="1">
+    </row>
+    <row r="22" spans="1:25" ht="15" customHeight="1">
       <c r="A22" s="36"/>
       <c r="B22" s="36"/>
       <c r="C22" s="36"/>
@@ -1897,9 +1877,8 @@
       <c r="W22" s="36"/>
       <c r="X22" s="36"/>
       <c r="Y22" s="36"/>
-      <c r="Z22" s="36"/>
-    </row>
-    <row r="23" spans="1:26" ht="15" customHeight="1">
+    </row>
+    <row r="23" spans="1:25" ht="15" customHeight="1">
       <c r="A23" s="36"/>
       <c r="B23" s="36"/>
       <c r="C23" s="36"/>
@@ -1925,9 +1904,8 @@
       <c r="W23" s="36"/>
       <c r="X23" s="36"/>
       <c r="Y23" s="36"/>
-      <c r="Z23" s="36"/>
-    </row>
-    <row r="24" spans="1:26" ht="15" customHeight="1">
+    </row>
+    <row r="24" spans="1:25" ht="15" customHeight="1">
       <c r="A24" s="36"/>
       <c r="B24" s="36"/>
       <c r="C24" s="36"/>
@@ -1953,9 +1931,8 @@
       <c r="W24" s="36"/>
       <c r="X24" s="36"/>
       <c r="Y24" s="36"/>
-      <c r="Z24" s="36"/>
-    </row>
-    <row r="25" spans="1:26" ht="15" customHeight="1">
+    </row>
+    <row r="25" spans="1:25" ht="15" customHeight="1">
       <c r="A25" s="36"/>
       <c r="B25" s="36"/>
       <c r="C25" s="36"/>
@@ -1981,7 +1958,6 @@
       <c r="W25" s="36"/>
       <c r="X25" s="36"/>
       <c r="Y25" s="36"/>
-      <c r="Z25" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1995,7 +1971,7 @@
   <phoneticPr fontId="3"/>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.39370078740157499" right="0.39370078740157499" top="0.98425196850393704" bottom="0.39370078740157499" header="0.39370078740157499" footer="0.31496062992126"/>
-  <pageSetup paperSize="9" scale="91" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="98" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;"MSゴシック,Regular"あいうえおあいうえおあいうえおあ株式会社
 &amp;C&amp;"MSゴシック,Regular"&amp;16★年間勤務表（1ヶ月）&amp;R&amp;"MSゴシック,Regular"&amp;D　&amp;T　

</xml_diff>